<commit_message>
update input data drpv2
</commit_message>
<xml_diff>
--- a/DRP_v2/input_data.xlsx
+++ b/DRP_v2/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F8AEDD-425B-471A-89AA-C4484CEE689D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C879820D-0B28-4BE3-8212-D79DEBF81FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rank_oct" sheetId="15" r:id="rId1"/>
@@ -44,7 +44,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -53,7 +53,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -68,7 +68,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -77,7 +77,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -102,7 +102,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -111,7 +111,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -126,7 +126,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -135,7 +135,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -150,7 +150,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -159,7 +159,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -184,7 +184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -193,7 +193,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -353,7 +353,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -362,7 +362,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -377,7 +377,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -386,7 +386,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Lead Time Dependent</t>
@@ -941,9 +941,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-14409]d\ mmmm\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14409]d\ mmmm\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1028,19 +1028,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2430,8 +2417,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="288">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2521,34 +2508,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2607,14 +2594,14 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="60" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="60" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="61" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="61" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="62" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="62" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2629,31 +2616,31 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2675,14 +2662,14 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2714,13 +2701,13 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2765,8 +2752,8 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2803,28 +2790,28 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="76" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="76" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="77" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="77" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="26" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="38" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="38" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="75" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2836,11 +2823,340 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="81" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="41" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="89" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="67" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="16" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="2" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="64" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="65" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="48" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2872,100 +3188,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="48" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="64" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="65" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2980,283 +3203,47 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="48" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="48" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="64" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="63" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="81" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="64" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="41" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="90" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="84" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="80" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="89" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="90" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="88" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="84" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="87" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="85" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="86" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="85" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="87" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="86" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="88" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="67" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -8121,7 +8108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44062F5F-0CA8-46B4-A3F3-D2A7A3B7D14D}">
   <dimension ref="C2:O86"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -9949,7 +9936,7 @@
       <c r="D86" s="31"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="54">
       <colorScale>
@@ -10739,7 +10726,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3F269F04-7808-4E61-9FC1-FB7CE107EE15}">
           <x14:formula1>
             <xm:f>Selection!$I$2:$I$10</xm:f>
@@ -12650,7 +12637,7 @@
       <c r="K86"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="I25">
     <cfRule type="colorScale" priority="54">
       <colorScale>
@@ -16181,7 +16168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AA01D1-3AF4-4CE2-8512-855E90452B9D}">
   <dimension ref="B2:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -16207,10 +16194,10 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="172" t="s">
+      <c r="D3" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="173"/>
+      <c r="E3" s="246"/>
       <c r="G3" t="s">
         <v>58</v>
       </c>
@@ -16271,11 +16258,11 @@
       <c r="H12" s="102"/>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L13" s="158" t="s">
+      <c r="L13" s="252" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="159"/>
-      <c r="N13" s="160"/>
+      <c r="M13" s="253"/>
+      <c r="N13" s="254"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G14" s="87" t="s">
@@ -16302,13 +16289,13 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="165" t="s">
+      <c r="F15" s="247" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="166" t="s">
+      <c r="G15" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="161" t="s">
+      <c r="H15" s="255" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="66" t="s">
@@ -16332,9 +16319,9 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="165"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="162"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="249"/>
+      <c r="H16" s="256"/>
       <c r="I16" s="67" t="s">
         <v>86</v>
       </c>
@@ -16353,11 +16340,11 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="165"/>
-      <c r="G17" s="168" t="s">
+      <c r="F17" s="247"/>
+      <c r="G17" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="163" t="s">
+      <c r="H17" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="68" t="s">
@@ -16381,9 +16368,9 @@
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="165"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="162"/>
+      <c r="F18" s="247"/>
+      <c r="G18" s="249"/>
+      <c r="H18" s="256"/>
       <c r="I18" s="67" t="s">
         <v>86</v>
       </c>
@@ -16402,11 +16389,11 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="165"/>
-      <c r="G19" s="168" t="s">
+      <c r="F19" s="247"/>
+      <c r="G19" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="163" t="s">
+      <c r="H19" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="68" t="s">
@@ -16430,9 +16417,9 @@
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="165"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="162"/>
+      <c r="F20" s="247"/>
+      <c r="G20" s="249"/>
+      <c r="H20" s="256"/>
       <c r="I20" s="67" t="s">
         <v>86</v>
       </c>
@@ -16451,11 +16438,11 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="165"/>
-      <c r="G21" s="168" t="s">
+      <c r="F21" s="247"/>
+      <c r="G21" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="163" t="s">
+      <c r="H21" s="257" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="65" t="s">
@@ -16479,9 +16466,9 @@
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="165"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="164"/>
+      <c r="F22" s="247"/>
+      <c r="G22" s="251"/>
+      <c r="H22" s="258"/>
       <c r="I22" s="67" t="s">
         <v>86</v>
       </c>
@@ -16544,10 +16531,10 @@
       </c>
     </row>
     <row r="25" spans="6:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="170" t="s">
+      <c r="G25" s="243" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="171"/>
+      <c r="H25" s="244"/>
       <c r="I25" s="93" t="s">
         <v>55</v>
       </c>
@@ -16566,10 +16553,10 @@
       </c>
     </row>
     <row r="26" spans="6:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="152" t="s">
+      <c r="G26" s="263" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="152"/>
+      <c r="H26" s="263"/>
       <c r="I26" s="12" t="s">
         <v>62</v>
       </c>
@@ -16592,8 +16579,8 @@
       </c>
     </row>
     <row r="27" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="152"/>
-      <c r="H27" s="152"/>
+      <c r="G27" s="263"/>
+      <c r="H27" s="263"/>
       <c r="I27" s="114" t="s">
         <v>61</v>
       </c>
@@ -16619,10 +16606,10 @@
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="153" t="s">
+      <c r="G28" s="264" t="s">
         <v>96</v>
       </c>
-      <c r="H28" s="153"/>
+      <c r="H28" s="264"/>
       <c r="I28" s="21" t="s">
         <v>62</v>
       </c>
@@ -16645,8 +16632,8 @@
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="153"/>
-      <c r="H29" s="153"/>
+      <c r="G29" s="264"/>
+      <c r="H29" s="264"/>
       <c r="I29" s="17" t="s">
         <v>61</v>
       </c>
@@ -16715,30 +16702,30 @@
     <row r="32" spans="6:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I32" s="107"/>
       <c r="J32" s="107"/>
-      <c r="K32" s="154" t="s">
+      <c r="K32" s="265" t="s">
         <v>92</v>
       </c>
-      <c r="L32" s="155"/>
-      <c r="M32" s="148" t="s">
+      <c r="L32" s="266"/>
+      <c r="M32" s="259" t="s">
         <v>89</v>
       </c>
-      <c r="N32" s="149"/>
+      <c r="N32" s="260"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.3">
       <c r="I33" s="107"/>
       <c r="J33" s="107"/>
-      <c r="K33" s="154"/>
-      <c r="L33" s="155"/>
-      <c r="M33" s="150"/>
-      <c r="N33" s="151"/>
+      <c r="K33" s="265"/>
+      <c r="L33" s="266"/>
+      <c r="M33" s="261"/>
+      <c r="N33" s="262"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.3">
       <c r="I34" s="107" t="s">
         <v>85</v>
       </c>
       <c r="J34" s="107"/>
-      <c r="K34" s="156"/>
-      <c r="L34" s="157"/>
+      <c r="K34" s="267"/>
+      <c r="L34" s="268"/>
       <c r="M34" s="108"/>
       <c r="N34" s="46"/>
     </row>
@@ -16782,11 +16769,11 @@
       <c r="H42" s="102"/>
     </row>
     <row r="43" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L43" s="158" t="s">
+      <c r="L43" s="252" t="s">
         <v>51</v>
       </c>
-      <c r="M43" s="159"/>
-      <c r="N43" s="160"/>
+      <c r="M43" s="253"/>
+      <c r="N43" s="254"/>
     </row>
     <row r="44" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G44" s="87" t="s">
@@ -16813,13 +16800,13 @@
       </c>
     </row>
     <row r="45" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F45" s="165" t="s">
+      <c r="F45" s="247" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="166" t="s">
+      <c r="G45" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="161" t="s">
+      <c r="H45" s="255" t="s">
         <v>9</v>
       </c>
       <c r="I45" s="66" t="s">
@@ -16843,9 +16830,9 @@
       </c>
     </row>
     <row r="46" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F46" s="165"/>
-      <c r="G46" s="167"/>
-      <c r="H46" s="162"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="249"/>
+      <c r="H46" s="256"/>
       <c r="I46" s="67" t="s">
         <v>86</v>
       </c>
@@ -16864,11 +16851,11 @@
       </c>
     </row>
     <row r="47" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F47" s="165"/>
-      <c r="G47" s="168" t="s">
+      <c r="F47" s="247"/>
+      <c r="G47" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="163" t="s">
+      <c r="H47" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I47" s="68" t="s">
@@ -16892,9 +16879,9 @@
       </c>
     </row>
     <row r="48" spans="3:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F48" s="165"/>
-      <c r="G48" s="167"/>
-      <c r="H48" s="162"/>
+      <c r="F48" s="247"/>
+      <c r="G48" s="249"/>
+      <c r="H48" s="256"/>
       <c r="I48" s="67" t="s">
         <v>86</v>
       </c>
@@ -16913,11 +16900,11 @@
       </c>
     </row>
     <row r="49" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F49" s="165"/>
-      <c r="G49" s="168" t="s">
+      <c r="F49" s="247"/>
+      <c r="G49" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="H49" s="163" t="s">
+      <c r="H49" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I49" s="68" t="s">
@@ -16941,9 +16928,9 @@
       </c>
     </row>
     <row r="50" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F50" s="165"/>
-      <c r="G50" s="167"/>
-      <c r="H50" s="162"/>
+      <c r="F50" s="247"/>
+      <c r="G50" s="249"/>
+      <c r="H50" s="256"/>
       <c r="I50" s="67" t="s">
         <v>86</v>
       </c>
@@ -16962,11 +16949,11 @@
       </c>
     </row>
     <row r="51" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F51" s="165"/>
-      <c r="G51" s="168" t="s">
+      <c r="F51" s="247"/>
+      <c r="G51" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="163" t="s">
+      <c r="H51" s="257" t="s">
         <v>12</v>
       </c>
       <c r="I51" s="65" t="s">
@@ -16990,9 +16977,9 @@
       </c>
     </row>
     <row r="52" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F52" s="165"/>
-      <c r="G52" s="169"/>
-      <c r="H52" s="164"/>
+      <c r="F52" s="247"/>
+      <c r="G52" s="251"/>
+      <c r="H52" s="258"/>
       <c r="I52" s="67" t="s">
         <v>86</v>
       </c>
@@ -17170,10 +17157,10 @@
       </c>
     </row>
     <row r="60" spans="3:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G60" s="170" t="s">
+      <c r="G60" s="243" t="s">
         <v>57</v>
       </c>
-      <c r="H60" s="171"/>
+      <c r="H60" s="244"/>
       <c r="I60" s="93" t="s">
         <v>55</v>
       </c>
@@ -17230,14 +17217,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F15:F22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="G26:H27"/>
+    <mergeCell ref="G28:H29"/>
+    <mergeCell ref="K32:L34"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H22"/>
     <mergeCell ref="L43:N43"/>
     <mergeCell ref="F45:F52"/>
     <mergeCell ref="G45:G46"/>
@@ -17248,15 +17236,14 @@
     <mergeCell ref="H49:H50"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="G26:H27"/>
-    <mergeCell ref="G28:H29"/>
-    <mergeCell ref="K32:L34"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F15:F22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17293,8 +17280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D7FAAB-7DDB-4E38-A93A-468347C2F4C1}">
   <dimension ref="B2:V81"/>
   <sheetViews>
-    <sheetView topLeftCell="I31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="I10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17320,10 +17307,10 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="172" t="s">
+      <c r="D3" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="173"/>
+      <c r="E3" s="246"/>
       <c r="G3" t="s">
         <v>58</v>
       </c>
@@ -17377,7 +17364,7 @@
       <c r="C9" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="196">
+      <c r="D9" s="165">
         <v>2400</v>
       </c>
       <c r="E9" t="s">
@@ -17401,11 +17388,11 @@
       <c r="H12" s="102"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M13" s="158" t="s">
+      <c r="M13" s="252" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="159"/>
-      <c r="O13" s="160"/>
+      <c r="N13" s="253"/>
+      <c r="O13" s="254"/>
     </row>
     <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G14" s="87" t="s">
@@ -17435,13 +17422,13 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="165" t="s">
+      <c r="F15" s="247" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="166" t="s">
+      <c r="G15" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="161" t="s">
+      <c r="H15" s="255" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="135" t="s">
@@ -17458,19 +17445,19 @@
         <f>rank_oct!$O$7</f>
         <v>1035</v>
       </c>
-      <c r="N15" s="197">
+      <c r="N15" s="166">
         <f>rank_nov!$O$7</f>
         <v>1025</v>
       </c>
-      <c r="O15" s="198">
+      <c r="O15" s="167">
         <f>rank_dec!$O$7</f>
         <v>975</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="165"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="162"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="249"/>
+      <c r="H16" s="256"/>
       <c r="I16" s="121" t="s">
         <v>86</v>
       </c>
@@ -17492,11 +17479,11 @@
       </c>
     </row>
     <row r="17" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="165"/>
-      <c r="G17" s="168" t="s">
+      <c r="F17" s="247"/>
+      <c r="G17" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="163" t="s">
+      <c r="H17" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="136" t="s">
@@ -17512,19 +17499,19 @@
       <c r="M17" s="63">
         <v>310</v>
       </c>
-      <c r="N17" s="199">
+      <c r="N17" s="168">
         <f>rank_nov!$O$8</f>
         <v>300</v>
       </c>
-      <c r="O17" s="200">
+      <c r="O17" s="169">
         <f>rank_dec!$O$8</f>
         <v>360</v>
       </c>
     </row>
     <row r="18" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="165"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="162"/>
+      <c r="F18" s="247"/>
+      <c r="G18" s="249"/>
+      <c r="H18" s="256"/>
       <c r="I18" s="121" t="s">
         <v>86</v>
       </c>
@@ -17546,11 +17533,11 @@
       </c>
     </row>
     <row r="19" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="165"/>
-      <c r="G19" s="168" t="s">
+      <c r="F19" s="247"/>
+      <c r="G19" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="163" t="s">
+      <c r="H19" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="136" t="s">
@@ -17567,19 +17554,19 @@
         <f>rank_oct!$O$9</f>
         <v>130</v>
       </c>
-      <c r="N19" s="199">
+      <c r="N19" s="168">
         <f>rank_nov!$O$9</f>
         <v>100</v>
       </c>
-      <c r="O19" s="200">
+      <c r="O19" s="169">
         <f>rank_dec!$O$9</f>
         <v>110</v>
       </c>
     </row>
     <row r="20" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="165"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="162"/>
+      <c r="F20" s="247"/>
+      <c r="G20" s="249"/>
+      <c r="H20" s="256"/>
       <c r="I20" s="121" t="s">
         <v>86</v>
       </c>
@@ -17601,11 +17588,11 @@
       </c>
     </row>
     <row r="21" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="165"/>
-      <c r="G21" s="168" t="s">
+      <c r="F21" s="247"/>
+      <c r="G21" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="163" t="s">
+      <c r="H21" s="257" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="136" t="s">
@@ -17622,19 +17609,19 @@
         <f>rank_oct!$O$10</f>
         <v>890</v>
       </c>
-      <c r="N21" s="199">
+      <c r="N21" s="168">
         <f>rank_nov!$O$10</f>
         <v>840</v>
       </c>
-      <c r="O21" s="200">
+      <c r="O21" s="169">
         <f>rank_dec!$O$10</f>
         <v>840</v>
       </c>
     </row>
     <row r="22" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="165"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="164"/>
+      <c r="F22" s="247"/>
+      <c r="G22" s="251"/>
+      <c r="H22" s="258"/>
       <c r="I22" s="122" t="s">
         <v>86</v>
       </c>
@@ -17671,11 +17658,11 @@
         <f t="shared" ref="M23:O23" si="0">M15+M17+M19+M21</f>
         <v>2365</v>
       </c>
-      <c r="N23" s="201">
+      <c r="N23" s="170">
         <f t="shared" si="0"/>
         <v>2265</v>
       </c>
-      <c r="O23" s="202">
+      <c r="O23" s="171">
         <f t="shared" si="0"/>
         <v>2285</v>
       </c>
@@ -17706,40 +17693,40 @@
       </c>
     </row>
     <row r="25" spans="6:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="195" t="s">
+      <c r="F25" s="274" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="237" t="s">
+      <c r="G25" s="274"/>
+      <c r="H25" s="274"/>
+      <c r="I25" s="200" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="238" t="s">
+      <c r="J25" s="201" t="s">
         <v>107</v>
       </c>
       <c r="K25" s="116"/>
-      <c r="L25" s="239">
+      <c r="L25" s="202">
         <v>2400</v>
       </c>
-      <c r="M25" s="239">
+      <c r="M25" s="202">
         <v>2400</v>
       </c>
-      <c r="N25" s="240">
+      <c r="N25" s="203">
         <v>2300</v>
       </c>
-      <c r="O25" s="241">
+      <c r="O25" s="204">
         <v>2300</v>
       </c>
     </row>
     <row r="26" spans="6:22" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="219" t="s">
+      <c r="G26" s="275" t="s">
         <v>149</v>
       </c>
-      <c r="H26" s="220"/>
+      <c r="H26" s="276"/>
       <c r="I26" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J26" s="210" t="s">
+      <c r="J26" s="178" t="s">
         <v>112</v>
       </c>
       <c r="K26" s="132"/>
@@ -17761,47 +17748,47 @@
       </c>
     </row>
     <row r="27" spans="6:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="219"/>
-      <c r="H27" s="220"/>
+      <c r="G27" s="275"/>
+      <c r="H27" s="276"/>
       <c r="I27" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="J27" s="211" t="s">
+      <c r="J27" s="179" t="s">
         <v>111</v>
       </c>
-      <c r="K27" s="205">
+      <c r="K27" s="174">
         <f>D7</f>
         <v>450</v>
       </c>
-      <c r="L27" s="206">
+      <c r="L27" s="175">
         <f>L26-L23</f>
         <v>385</v>
       </c>
-      <c r="M27" s="206">
+      <c r="M27" s="175">
         <f t="shared" ref="M27:O27" si="3">M26-M23</f>
         <v>420</v>
       </c>
-      <c r="N27" s="206">
+      <c r="N27" s="175">
         <f t="shared" si="3"/>
         <v>455</v>
       </c>
-      <c r="O27" s="207">
+      <c r="O27" s="176">
         <f t="shared" si="3"/>
         <v>470</v>
       </c>
     </row>
     <row r="28" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="G28" s="217" t="s">
+      <c r="G28" s="277" t="s">
         <v>137</v>
       </c>
-      <c r="H28" s="218"/>
+      <c r="H28" s="278"/>
       <c r="I28" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J28" s="188" t="s">
+      <c r="J28" s="162" t="s">
         <v>113</v>
       </c>
-      <c r="K28" s="213"/>
+      <c r="K28" s="181"/>
       <c r="L28" s="27">
         <f>K30+L25</f>
         <v>2850</v>
@@ -17820,8 +17807,8 @@
       </c>
     </row>
     <row r="29" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="G29" s="217"/>
-      <c r="H29" s="218"/>
+      <c r="G29" s="277"/>
+      <c r="H29" s="278"/>
       <c r="I29" s="21"/>
       <c r="J29" s="143"/>
       <c r="K29" s="133"/>
@@ -17834,15 +17821,15 @@
       <c r="O29" s="111"/>
     </row>
     <row r="30" spans="6:22" x14ac:dyDescent="0.3">
-      <c r="G30" s="217"/>
-      <c r="H30" s="218"/>
+      <c r="G30" s="277"/>
+      <c r="H30" s="278"/>
       <c r="I30" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="216" t="s">
+      <c r="J30" s="184" t="s">
         <v>114</v>
       </c>
-      <c r="K30" s="214">
+      <c r="K30" s="182">
         <f>D7</f>
         <v>450</v>
       </c>
@@ -17871,14 +17858,14 @@
       <c r="I31" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="J31" s="216" t="s">
+      <c r="J31" s="184" t="s">
         <v>116</v>
       </c>
-      <c r="K31" s="215"/>
-      <c r="L31" s="236" t="s">
+      <c r="K31" s="183"/>
+      <c r="L31" s="199" t="s">
         <v>148</v>
       </c>
-      <c r="M31" s="236" t="s">
+      <c r="M31" s="199" t="s">
         <v>148</v>
       </c>
       <c r="N31" s="5">
@@ -17922,19 +17909,19 @@
       </c>
     </row>
     <row r="33" spans="3:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F33" s="195" t="s">
+      <c r="F33" s="274" t="s">
         <v>129</v>
       </c>
-      <c r="G33" s="195"/>
-      <c r="H33" s="209"/>
-      <c r="I33" s="212" t="s">
+      <c r="G33" s="274"/>
+      <c r="H33" s="279"/>
+      <c r="I33" s="180" t="s">
         <v>121</v>
       </c>
-      <c r="J33" s="208" t="s">
+      <c r="J33" s="177" t="s">
         <v>122</v>
       </c>
       <c r="K33" s="123"/>
-      <c r="L33" s="189"/>
+      <c r="L33" s="163"/>
       <c r="M33" s="95">
         <v>2400</v>
       </c>
@@ -17942,7 +17929,7 @@
         <f>N25-L32</f>
         <v>2235</v>
       </c>
-      <c r="O33" s="194">
+      <c r="O33" s="164">
         <f>O25-M32</f>
         <v>-130</v>
       </c>
@@ -17951,29 +17938,29 @@
       </c>
     </row>
     <row r="34" spans="3:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E34" s="225" t="s">
+      <c r="E34" s="269" t="s">
         <v>134</v>
       </c>
-      <c r="F34" s="225"/>
-      <c r="G34" s="225"/>
-      <c r="H34" s="225"/>
-      <c r="I34" s="203" t="s">
+      <c r="F34" s="269"/>
+      <c r="G34" s="269"/>
+      <c r="H34" s="269"/>
+      <c r="I34" s="172" t="s">
         <v>133</v>
       </c>
-      <c r="J34" s="222" t="s">
+      <c r="J34" s="186" t="s">
         <v>131</v>
       </c>
-      <c r="K34" s="203"/>
-      <c r="L34" s="204"/>
-      <c r="M34" s="223">
+      <c r="K34" s="172"/>
+      <c r="L34" s="173"/>
+      <c r="M34" s="187">
         <f>IF(M33&gt;$D$9, M33 - $D$9, 0)</f>
         <v>0</v>
       </c>
-      <c r="N34" s="221">
+      <c r="N34" s="185">
         <f t="shared" ref="N34:O34" si="5">IF(N33&gt;$D$9, N33 - $D$9, 0)</f>
         <v>0</v>
       </c>
-      <c r="O34" s="224">
+      <c r="O34" s="188">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -17985,14 +17972,14 @@
       <c r="I35" s="107"/>
       <c r="J35" s="107"/>
       <c r="K35" s="107"/>
-      <c r="L35" s="154" t="s">
+      <c r="L35" s="265" t="s">
         <v>92</v>
       </c>
-      <c r="M35" s="155"/>
-      <c r="N35" s="190" t="s">
+      <c r="M35" s="266"/>
+      <c r="N35" s="270" t="s">
         <v>89</v>
       </c>
-      <c r="O35" s="191"/>
+      <c r="O35" s="271"/>
       <c r="R35" t="s">
         <v>153</v>
       </c>
@@ -18001,10 +17988,10 @@
       <c r="I36" s="107"/>
       <c r="J36" s="107"/>
       <c r="K36" s="107"/>
-      <c r="L36" s="154"/>
-      <c r="M36" s="155"/>
-      <c r="N36" s="192"/>
-      <c r="O36" s="193"/>
+      <c r="L36" s="265"/>
+      <c r="M36" s="266"/>
+      <c r="N36" s="272"/>
+      <c r="O36" s="273"/>
       <c r="R36" t="s">
         <v>162</v>
       </c>
@@ -18013,8 +18000,8 @@
       <c r="I37" s="107"/>
       <c r="J37" s="107"/>
       <c r="K37" s="107"/>
-      <c r="L37" s="156"/>
-      <c r="M37" s="157"/>
+      <c r="L37" s="267"/>
+      <c r="M37" s="268"/>
       <c r="N37" s="108"/>
       <c r="O37" s="46"/>
       <c r="S37" t="s">
@@ -18048,7 +18035,7 @@
       <c r="C42" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="178">
+      <c r="D42" s="152">
         <v>500</v>
       </c>
       <c r="E42" t="s">
@@ -18063,7 +18050,7 @@
       <c r="C43" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="179">
+      <c r="D43" s="153">
         <v>50</v>
       </c>
       <c r="E43" t="s">
@@ -18081,7 +18068,7 @@
       <c r="C44" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="179">
+      <c r="D44" s="153">
         <v>1</v>
       </c>
       <c r="E44" t="s">
@@ -18099,7 +18086,7 @@
       <c r="C45" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="196">
+      <c r="D45" s="165">
         <v>2400</v>
       </c>
       <c r="E45" t="s">
@@ -18116,11 +18103,11 @@
     </row>
     <row r="46" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J46" s="1"/>
-      <c r="M46" s="158" t="s">
+      <c r="M46" s="252" t="s">
         <v>51</v>
       </c>
-      <c r="N46" s="159"/>
-      <c r="O46" s="160"/>
+      <c r="N46" s="253"/>
+      <c r="O46" s="254"/>
     </row>
     <row r="47" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G47" s="87" t="s">
@@ -18150,13 +18137,13 @@
       </c>
     </row>
     <row r="48" spans="3:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F48" s="165" t="s">
+      <c r="F48" s="247" t="s">
         <v>56</v>
       </c>
-      <c r="G48" s="166" t="s">
+      <c r="G48" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="161" t="s">
+      <c r="H48" s="255" t="s">
         <v>9</v>
       </c>
       <c r="I48" s="135" t="s">
@@ -18184,9 +18171,9 @@
       </c>
     </row>
     <row r="49" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F49" s="165"/>
-      <c r="G49" s="167"/>
-      <c r="H49" s="162"/>
+      <c r="F49" s="247"/>
+      <c r="G49" s="249"/>
+      <c r="H49" s="256"/>
       <c r="I49" s="121" t="s">
         <v>86</v>
       </c>
@@ -18208,11 +18195,11 @@
       </c>
     </row>
     <row r="50" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F50" s="165"/>
-      <c r="G50" s="168" t="s">
+      <c r="F50" s="247"/>
+      <c r="G50" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H50" s="163" t="s">
+      <c r="H50" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I50" s="136" t="s">
@@ -18230,19 +18217,19 @@
         <f>rank_oct!$O$8</f>
         <v>310</v>
       </c>
-      <c r="N50" s="174">
+      <c r="N50" s="148">
         <f>rank_nov!$O$8</f>
         <v>300</v>
       </c>
-      <c r="O50" s="175">
+      <c r="O50" s="149">
         <f>rank_dec!$O$8</f>
         <v>360</v>
       </c>
     </row>
     <row r="51" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F51" s="165"/>
-      <c r="G51" s="167"/>
-      <c r="H51" s="162"/>
+      <c r="F51" s="247"/>
+      <c r="G51" s="249"/>
+      <c r="H51" s="256"/>
       <c r="I51" s="121" t="s">
         <v>86</v>
       </c>
@@ -18264,11 +18251,11 @@
       </c>
     </row>
     <row r="52" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F52" s="165"/>
-      <c r="G52" s="168" t="s">
+      <c r="F52" s="247"/>
+      <c r="G52" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="H52" s="163" t="s">
+      <c r="H52" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I52" s="136" t="s">
@@ -18286,19 +18273,19 @@
         <f>rank_oct!$O$9</f>
         <v>130</v>
       </c>
-      <c r="N52" s="174">
+      <c r="N52" s="148">
         <f>rank_nov!$O$9</f>
         <v>100</v>
       </c>
-      <c r="O52" s="175">
+      <c r="O52" s="149">
         <f>rank_dec!$O$9</f>
         <v>110</v>
       </c>
     </row>
     <row r="53" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F53" s="165"/>
-      <c r="G53" s="167"/>
-      <c r="H53" s="162"/>
+      <c r="F53" s="247"/>
+      <c r="G53" s="249"/>
+      <c r="H53" s="256"/>
       <c r="I53" s="121" t="s">
         <v>86</v>
       </c>
@@ -18320,11 +18307,11 @@
       </c>
     </row>
     <row r="54" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F54" s="165"/>
-      <c r="G54" s="168" t="s">
+      <c r="F54" s="247"/>
+      <c r="G54" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="163" t="s">
+      <c r="H54" s="257" t="s">
         <v>12</v>
       </c>
       <c r="I54" s="136" t="s">
@@ -18342,19 +18329,19 @@
         <f>rank_oct!$O$10</f>
         <v>890</v>
       </c>
-      <c r="N54" s="174">
+      <c r="N54" s="148">
         <f>rank_nov!$O$10</f>
         <v>840</v>
       </c>
-      <c r="O54" s="175">
+      <c r="O54" s="149">
         <f>rank_dec!$O$10</f>
         <v>840</v>
       </c>
     </row>
     <row r="55" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F55" s="165"/>
-      <c r="G55" s="169"/>
-      <c r="H55" s="164"/>
+      <c r="F55" s="247"/>
+      <c r="G55" s="251"/>
+      <c r="H55" s="258"/>
       <c r="I55" s="122" t="s">
         <v>86</v>
       </c>
@@ -18391,11 +18378,11 @@
         <f t="shared" ref="M56:O57" si="6">M48+M50+M52+M54</f>
         <v>2365</v>
       </c>
-      <c r="N56" s="176">
+      <c r="N56" s="150">
         <f t="shared" si="6"/>
         <v>2265</v>
       </c>
-      <c r="O56" s="177">
+      <c r="O56" s="151">
         <f t="shared" si="6"/>
         <v>2285</v>
       </c>
@@ -18407,20 +18394,20 @@
       <c r="J57" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="K57" s="184"/>
-      <c r="L57" s="185">
+      <c r="K57" s="158"/>
+      <c r="L57" s="159">
         <f>L49+L51+L53+L55</f>
         <v>2000</v>
       </c>
-      <c r="M57" s="186">
+      <c r="M57" s="160">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N57" s="186">
+      <c r="N57" s="160">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O57" s="187">
+      <c r="O57" s="161">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -18429,35 +18416,35 @@
       <c r="H58" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="I58" s="227" t="s">
+      <c r="I58" s="190" t="s">
         <v>142</v>
       </c>
-      <c r="J58" s="228" t="s">
+      <c r="J58" s="191" t="s">
         <v>120</v>
       </c>
-      <c r="K58" s="229"/>
-      <c r="L58" s="230">
+      <c r="K58" s="192"/>
+      <c r="L58" s="193">
         <v>300</v>
       </c>
-      <c r="M58" s="230">
+      <c r="M58" s="193">
         <v>200</v>
       </c>
-      <c r="N58" s="230">
+      <c r="N58" s="193">
         <v>300</v>
       </c>
-      <c r="O58" s="231">
+      <c r="O58" s="194">
         <v>200</v>
       </c>
     </row>
     <row r="59" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G59" s="152" t="s">
+      <c r="G59" s="263" t="s">
         <v>136</v>
       </c>
-      <c r="H59" s="152"/>
+      <c r="H59" s="263"/>
       <c r="I59" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J59" s="188" t="s">
+      <c r="J59" s="162" t="s">
         <v>141</v>
       </c>
       <c r="K59" s="99"/>
@@ -18479,12 +18466,12 @@
       </c>
     </row>
     <row r="60" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G60" s="152"/>
-      <c r="H60" s="152"/>
+      <c r="G60" s="263"/>
+      <c r="H60" s="263"/>
       <c r="I60" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J60" s="216" t="s">
+      <c r="J60" s="184" t="s">
         <v>111</v>
       </c>
       <c r="K60" s="58">
@@ -18509,12 +18496,12 @@
       </c>
     </row>
     <row r="61" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G61" s="152"/>
-      <c r="H61" s="152"/>
+      <c r="G61" s="263"/>
+      <c r="H61" s="263"/>
       <c r="I61" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="J61" s="226" t="s">
+      <c r="J61" s="189" t="s">
         <v>140</v>
       </c>
       <c r="K61" s="98"/>
@@ -18536,10 +18523,10 @@
       </c>
     </row>
     <row r="62" spans="6:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G62" s="170" t="s">
+      <c r="G62" s="243" t="s">
         <v>143</v>
       </c>
-      <c r="H62" s="171"/>
+      <c r="H62" s="244"/>
       <c r="I62" s="93" t="s">
         <v>55</v>
       </c>
@@ -18547,32 +18534,32 @@
         <v>145</v>
       </c>
       <c r="K62" s="94"/>
-      <c r="L62" s="180">
+      <c r="L62" s="154">
         <f xml:space="preserve"> CEILING(L61/$D$43,1)*$D$43</f>
         <v>2300</v>
       </c>
-      <c r="M62" s="180">
+      <c r="M62" s="154">
         <f t="shared" ref="M62:O62" si="10" xml:space="preserve"> CEILING(M61/$D$43,1)*$D$43</f>
         <v>2250</v>
       </c>
-      <c r="N62" s="232">
+      <c r="N62" s="195">
         <f t="shared" si="10"/>
         <v>2350</v>
       </c>
-      <c r="O62" s="194">
+      <c r="O62" s="164">
         <f t="shared" si="10"/>
         <v>2200</v>
       </c>
     </row>
     <row r="63" spans="6:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G63" s="152" t="s">
+      <c r="G63" s="263" t="s">
         <v>138</v>
       </c>
-      <c r="H63" s="152"/>
+      <c r="H63" s="263"/>
       <c r="I63" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J63" s="188" t="s">
+      <c r="J63" s="162" t="s">
         <v>113</v>
       </c>
       <c r="K63" s="99"/>
@@ -18594,12 +18581,12 @@
       </c>
     </row>
     <row r="64" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G64" s="152"/>
-      <c r="H64" s="152"/>
+      <c r="G64" s="263"/>
+      <c r="H64" s="263"/>
       <c r="I64" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J64" s="216" t="s">
+      <c r="J64" s="184" t="s">
         <v>114</v>
       </c>
       <c r="K64" s="58">
@@ -18624,19 +18611,19 @@
       </c>
     </row>
     <row r="65" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G65" s="152"/>
-      <c r="H65" s="152"/>
+      <c r="G65" s="263"/>
+      <c r="H65" s="263"/>
       <c r="I65" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="J65" s="226" t="s">
+      <c r="J65" s="189" t="s">
         <v>139</v>
       </c>
       <c r="K65" s="98"/>
-      <c r="L65" s="235" t="s">
+      <c r="L65" s="198" t="s">
         <v>148</v>
       </c>
-      <c r="M65" s="235" t="s">
+      <c r="M65" s="198" t="s">
         <v>148</v>
       </c>
       <c r="N65" s="23">
@@ -18649,10 +18636,10 @@
       </c>
     </row>
     <row r="66" spans="3:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G66" s="170" t="s">
+      <c r="G66" s="243" t="s">
         <v>144</v>
       </c>
-      <c r="H66" s="171"/>
+      <c r="H66" s="244"/>
       <c r="I66" s="93" t="s">
         <v>55</v>
       </c>
@@ -18660,19 +18647,19 @@
         <v>146</v>
       </c>
       <c r="K66" s="94"/>
-      <c r="L66" s="180">
+      <c r="L66" s="154">
         <f>L62</f>
         <v>2300</v>
       </c>
-      <c r="M66" s="180">
+      <c r="M66" s="154">
         <f>M62</f>
         <v>2250</v>
       </c>
-      <c r="N66" s="233">
+      <c r="N66" s="196">
         <f xml:space="preserve"> CEILING(N65/$D$43,1)*$D$43</f>
         <v>1900</v>
       </c>
-      <c r="O66" s="194">
+      <c r="O66" s="164">
         <f xml:space="preserve"> CEILING(O65/$D$43,1)*$D$43</f>
         <v>2200</v>
       </c>
@@ -18684,65 +18671,65 @@
       <c r="J67" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="K67" s="181"/>
-      <c r="L67" s="234">
+      <c r="K67" s="155"/>
+      <c r="L67" s="197">
         <f>M66</f>
         <v>2250</v>
       </c>
-      <c r="M67" s="182">
+      <c r="M67" s="156">
         <f t="shared" ref="M67:O67" si="14">N66</f>
         <v>1900</v>
       </c>
-      <c r="N67" s="182">
+      <c r="N67" s="156">
         <f t="shared" si="14"/>
         <v>2200</v>
       </c>
-      <c r="O67" s="183">
+      <c r="O67" s="157">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E68" s="225" t="s">
+      <c r="E68" s="269" t="s">
         <v>134</v>
       </c>
-      <c r="F68" s="225"/>
-      <c r="G68" s="225"/>
-      <c r="H68" s="225"/>
-      <c r="I68" s="203" t="s">
+      <c r="F68" s="269"/>
+      <c r="G68" s="269"/>
+      <c r="H68" s="269"/>
+      <c r="I68" s="172" t="s">
         <v>133</v>
       </c>
-      <c r="J68" s="222" t="s">
+      <c r="J68" s="186" t="s">
         <v>131</v>
       </c>
-      <c r="K68" s="203"/>
-      <c r="L68" s="204"/>
-      <c r="M68" s="223">
+      <c r="K68" s="172"/>
+      <c r="L68" s="173"/>
+      <c r="M68" s="187">
         <f>IF(M66&gt;$D$45, M66 - $D$45, 0)</f>
         <v>0</v>
       </c>
-      <c r="N68" s="221">
+      <c r="N68" s="185">
         <f>IF(N66&gt;$D$45, N66 - $D$45, 0)</f>
         <v>0</v>
       </c>
-      <c r="O68" s="224">
+      <c r="O68" s="188">
         <f>IF(O66&gt;$D$45, O66 - $D$45, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="L69" s="154" t="s">
+      <c r="L69" s="265" t="s">
         <v>92</v>
       </c>
-      <c r="M69" s="155"/>
+      <c r="M69" s="266"/>
     </row>
     <row r="70" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="L70" s="154"/>
-      <c r="M70" s="155"/>
+      <c r="L70" s="265"/>
+      <c r="M70" s="266"/>
     </row>
     <row r="71" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="L71" s="156"/>
-      <c r="M71" s="157"/>
+      <c r="L71" s="267"/>
+      <c r="M71" s="268"/>
     </row>
     <row r="79" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
@@ -18770,29 +18757,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E68:H68"/>
-    <mergeCell ref="L69:M71"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="G59:H61"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G63:H65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="L35:M37"/>
-    <mergeCell ref="N35:O36"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="F48:F55"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="G26:H27"/>
-    <mergeCell ref="G28:H30"/>
-    <mergeCell ref="F33:H33"/>
     <mergeCell ref="E34:H34"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="M13:O13"/>
@@ -18804,6 +18768,29 @@
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="G26:H27"/>
+    <mergeCell ref="G28:H30"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="L35:M37"/>
+    <mergeCell ref="N35:O36"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="F48:F55"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="L69:M71"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="G59:H61"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G63:H65"/>
+    <mergeCell ref="G66:H66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18840,8 +18827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FA8E5F-36E6-45D9-890A-FDD61C3D2B9D}">
   <dimension ref="B2:V99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N67" sqref="N67"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18867,10 +18854,10 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="172" t="s">
+      <c r="D3" s="245" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="173"/>
+      <c r="E3" s="246"/>
       <c r="G3" t="s">
         <v>58</v>
       </c>
@@ -18924,7 +18911,7 @@
       <c r="C9" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="196">
+      <c r="D9" s="165">
         <v>2400</v>
       </c>
       <c r="E9" t="s">
@@ -18948,11 +18935,11 @@
       <c r="H12" s="102"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M13" s="158" t="s">
+      <c r="M13" s="252" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="159"/>
-      <c r="O13" s="160"/>
+      <c r="N13" s="253"/>
+      <c r="O13" s="254"/>
     </row>
     <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G14" s="87" t="s">
@@ -18982,13 +18969,13 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F15" s="165" t="s">
+      <c r="F15" s="247" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="166" t="s">
+      <c r="G15" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="161" t="s">
+      <c r="H15" s="255" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="135" t="s">
@@ -19005,19 +18992,19 @@
         <f>rank_oct!$O$7</f>
         <v>1035</v>
       </c>
-      <c r="N15" s="197">
+      <c r="N15" s="166">
         <f>rank_nov!$O$7</f>
         <v>1025</v>
       </c>
-      <c r="O15" s="198">
+      <c r="O15" s="167">
         <f>rank_dec!$O$7</f>
         <v>975</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="165"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="162"/>
+      <c r="F16" s="247"/>
+      <c r="G16" s="249"/>
+      <c r="H16" s="256"/>
       <c r="I16" s="121" t="s">
         <v>86</v>
       </c>
@@ -19039,11 +19026,11 @@
       </c>
     </row>
     <row r="17" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="165"/>
-      <c r="G17" s="168" t="s">
+      <c r="F17" s="247"/>
+      <c r="G17" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="163" t="s">
+      <c r="H17" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="136" t="s">
@@ -19059,19 +19046,19 @@
       <c r="M17" s="63">
         <v>310</v>
       </c>
-      <c r="N17" s="199">
+      <c r="N17" s="168">
         <f>rank_nov!$O$8</f>
         <v>300</v>
       </c>
-      <c r="O17" s="200">
+      <c r="O17" s="169">
         <f>rank_dec!$O$8</f>
         <v>360</v>
       </c>
     </row>
     <row r="18" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="165"/>
-      <c r="G18" s="167"/>
-      <c r="H18" s="162"/>
+      <c r="F18" s="247"/>
+      <c r="G18" s="249"/>
+      <c r="H18" s="256"/>
       <c r="I18" s="121" t="s">
         <v>86</v>
       </c>
@@ -19093,11 +19080,11 @@
       </c>
     </row>
     <row r="19" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F19" s="165"/>
-      <c r="G19" s="168" t="s">
+      <c r="F19" s="247"/>
+      <c r="G19" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="163" t="s">
+      <c r="H19" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="136" t="s">
@@ -19114,19 +19101,19 @@
         <f>rank_oct!$O$9</f>
         <v>130</v>
       </c>
-      <c r="N19" s="199">
+      <c r="N19" s="168">
         <f>rank_nov!$O$9</f>
         <v>100</v>
       </c>
-      <c r="O19" s="200">
+      <c r="O19" s="169">
         <f>rank_dec!$O$9</f>
         <v>110</v>
       </c>
     </row>
     <row r="20" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="165"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="162"/>
+      <c r="F20" s="247"/>
+      <c r="G20" s="249"/>
+      <c r="H20" s="256"/>
       <c r="I20" s="121" t="s">
         <v>86</v>
       </c>
@@ -19148,11 +19135,11 @@
       </c>
     </row>
     <row r="21" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="165"/>
-      <c r="G21" s="168" t="s">
+      <c r="F21" s="247"/>
+      <c r="G21" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="163" t="s">
+      <c r="H21" s="257" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="136" t="s">
@@ -19169,19 +19156,19 @@
         <f>rank_oct!$O$10</f>
         <v>890</v>
       </c>
-      <c r="N21" s="199">
+      <c r="N21" s="168">
         <f>rank_nov!$O$10</f>
         <v>840</v>
       </c>
-      <c r="O21" s="200">
+      <c r="O21" s="169">
         <f>rank_dec!$O$10</f>
         <v>840</v>
       </c>
     </row>
     <row r="22" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="165"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="164"/>
+      <c r="F22" s="247"/>
+      <c r="G22" s="251"/>
+      <c r="H22" s="258"/>
       <c r="I22" s="122" t="s">
         <v>86</v>
       </c>
@@ -19218,11 +19205,11 @@
         <f t="shared" ref="M23:O23" si="0">M15+M17+M19+M21</f>
         <v>2365</v>
       </c>
-      <c r="N23" s="201">
+      <c r="N23" s="170">
         <f t="shared" si="0"/>
         <v>2265</v>
       </c>
-      <c r="O23" s="202">
+      <c r="O23" s="171">
         <f t="shared" si="0"/>
         <v>2285</v>
       </c>
@@ -19253,40 +19240,40 @@
       </c>
     </row>
     <row r="25" spans="6:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="195" t="s">
+      <c r="F25" s="274" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="237" t="s">
+      <c r="G25" s="274"/>
+      <c r="H25" s="274"/>
+      <c r="I25" s="200" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="238" t="s">
+      <c r="J25" s="201" t="s">
         <v>107</v>
       </c>
       <c r="K25" s="116"/>
-      <c r="L25" s="239">
+      <c r="L25" s="202">
         <v>2350</v>
       </c>
-      <c r="M25" s="239">
+      <c r="M25" s="202">
         <v>2350</v>
       </c>
-      <c r="N25" s="240">
+      <c r="N25" s="203">
         <v>2300</v>
       </c>
-      <c r="O25" s="261" t="s">
+      <c r="O25" s="216" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="26" spans="6:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="252" t="s">
+      <c r="G26" s="284" t="s">
         <v>171</v>
       </c>
-      <c r="H26" s="253"/>
+      <c r="H26" s="285"/>
       <c r="I26" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="J26" s="210" t="s">
+      <c r="J26" s="178" t="s">
         <v>166</v>
       </c>
       <c r="K26" s="10"/>
@@ -19302,20 +19289,20 @@
         <f t="shared" si="2"/>
         <v>2620</v>
       </c>
-      <c r="O26" s="257" t="s">
+      <c r="O26" s="212" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="27" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G27" s="250"/>
-      <c r="H27" s="251"/>
+      <c r="G27" s="286"/>
+      <c r="H27" s="287"/>
       <c r="I27" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="J27" s="242" t="s">
+      <c r="J27" s="205" t="s">
         <v>167</v>
       </c>
-      <c r="K27" s="245">
+      <c r="K27" s="208">
         <v>450</v>
       </c>
       <c r="L27" s="9">
@@ -19330,245 +19317,245 @@
         <f t="shared" si="3"/>
         <v>355</v>
       </c>
-      <c r="O27" s="258" t="s">
+      <c r="O27" s="213" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="28" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="250"/>
-      <c r="H28" s="251"/>
+      <c r="G28" s="286"/>
+      <c r="H28" s="287"/>
       <c r="I28" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J28" s="242" t="s">
+      <c r="J28" s="205" t="s">
         <v>168</v>
       </c>
-      <c r="K28" s="244"/>
-      <c r="L28" s="243">
+      <c r="K28" s="207"/>
+      <c r="L28" s="206">
         <f>K27-$D$8</f>
         <v>250</v>
       </c>
-      <c r="M28" s="243">
+      <c r="M28" s="206">
         <f t="shared" ref="M28:N28" si="4">L27-$D$8</f>
         <v>135</v>
       </c>
-      <c r="N28" s="243">
+      <c r="N28" s="206">
         <f t="shared" si="4"/>
         <v>120</v>
       </c>
-      <c r="O28" s="259" t="s">
+      <c r="O28" s="214" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="29" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="250"/>
-      <c r="H29" s="251"/>
+      <c r="G29" s="286"/>
+      <c r="H29" s="287"/>
       <c r="I29" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="J29" s="211" t="s">
+      <c r="J29" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="K29" s="244"/>
-      <c r="L29" s="243">
+      <c r="K29" s="207"/>
+      <c r="L29" s="206">
         <f>L25+L28</f>
         <v>2600</v>
       </c>
-      <c r="M29" s="243">
+      <c r="M29" s="206">
         <f>M25+M28</f>
         <v>2485</v>
       </c>
-      <c r="N29" s="243">
+      <c r="N29" s="206">
         <f>N25+N28</f>
         <v>2420</v>
       </c>
-      <c r="O29" s="259" t="s">
+      <c r="O29" s="214" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="30" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G30" s="254"/>
-      <c r="H30" s="255"/>
+      <c r="G30" s="282"/>
+      <c r="H30" s="283"/>
       <c r="I30" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="J30" s="256" t="s">
+      <c r="J30" s="211" t="s">
         <v>172</v>
       </c>
-      <c r="K30" s="246"/>
-      <c r="L30" s="247">
+      <c r="K30" s="209"/>
+      <c r="L30" s="210">
         <f>L29-L23</f>
         <v>135</v>
       </c>
-      <c r="M30" s="247">
+      <c r="M30" s="210">
         <f t="shared" ref="M30:N30" si="5">M29-M23</f>
         <v>120</v>
       </c>
-      <c r="N30" s="247">
+      <c r="N30" s="210">
         <f t="shared" si="5"/>
         <v>155</v>
       </c>
-      <c r="O30" s="260" t="s">
+      <c r="O30" s="215" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="31" spans="6:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G31" s="248" t="s">
+      <c r="G31" s="280" t="s">
         <v>137</v>
       </c>
-      <c r="H31" s="249"/>
+      <c r="H31" s="281"/>
       <c r="I31" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J31" s="262" t="s">
+      <c r="J31" s="217" t="s">
         <v>113</v>
       </c>
-      <c r="K31" s="263"/>
-      <c r="L31" s="264">
+      <c r="K31" s="218"/>
+      <c r="L31" s="219">
         <f>L26</f>
         <v>2800</v>
       </c>
-      <c r="M31" s="264">
+      <c r="M31" s="219">
         <f>L32+M37</f>
         <v>2750</v>
       </c>
-      <c r="N31" s="264">
+      <c r="N31" s="219">
         <f>M32+N37</f>
         <v>2620</v>
       </c>
-      <c r="O31" s="283">
+      <c r="O31" s="238">
         <f>N32+O37</f>
         <v>2555</v>
       </c>
     </row>
     <row r="32" spans="6:15" x14ac:dyDescent="0.3">
-      <c r="G32" s="254"/>
-      <c r="H32" s="255"/>
-      <c r="I32" s="265" t="s">
+      <c r="G32" s="282"/>
+      <c r="H32" s="283"/>
+      <c r="I32" s="220" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="266" t="s">
+      <c r="J32" s="221" t="s">
         <v>114</v>
       </c>
-      <c r="K32" s="267"/>
+      <c r="K32" s="222"/>
       <c r="L32" s="26">
         <f>L31-L24</f>
         <v>400</v>
       </c>
-      <c r="M32" s="268">
+      <c r="M32" s="223">
         <f>M31-M23</f>
         <v>385</v>
       </c>
-      <c r="N32" s="268">
+      <c r="N32" s="223">
         <f>N31-N23</f>
         <v>355</v>
       </c>
-      <c r="O32" s="269">
+      <c r="O32" s="224">
         <f>O31-O23</f>
         <v>270</v>
       </c>
     </row>
     <row r="33" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I33" s="265" t="s">
+      <c r="I33" s="220" t="s">
         <v>164</v>
       </c>
-      <c r="J33" s="280" t="s">
+      <c r="J33" s="235" t="s">
         <v>173</v>
       </c>
-      <c r="K33" s="270"/>
-      <c r="L33" s="268" t="s">
+      <c r="K33" s="225"/>
+      <c r="L33" s="223" t="s">
         <v>148</v>
       </c>
-      <c r="M33" s="268">
+      <c r="M33" s="223">
         <f>L32-$D$8</f>
         <v>200</v>
       </c>
-      <c r="N33" s="268">
+      <c r="N33" s="223">
         <f t="shared" ref="N33:O33" si="6">M32-$D$8</f>
         <v>185</v>
       </c>
-      <c r="O33" s="269">
+      <c r="O33" s="224">
         <f t="shared" si="6"/>
         <v>155</v>
       </c>
     </row>
     <row r="34" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I34" s="265" t="s">
+      <c r="I34" s="220" t="s">
         <v>165</v>
       </c>
-      <c r="J34" s="281" t="s">
+      <c r="J34" s="236" t="s">
         <v>174</v>
       </c>
-      <c r="K34" s="270"/>
-      <c r="L34" s="268" t="s">
+      <c r="K34" s="225"/>
+      <c r="L34" s="223" t="s">
         <v>148</v>
       </c>
-      <c r="M34" s="268">
+      <c r="M34" s="223">
         <f>M33+M25</f>
         <v>2550</v>
       </c>
-      <c r="N34" s="268">
+      <c r="N34" s="223">
         <f>N33+N37</f>
         <v>2420</v>
       </c>
-      <c r="O34" s="269">
+      <c r="O34" s="224">
         <f>O33+O37</f>
         <v>2355</v>
       </c>
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I35" s="265" t="s">
+      <c r="I35" s="220" t="s">
         <v>80</v>
       </c>
-      <c r="J35" s="266" t="s">
+      <c r="J35" s="221" t="s">
         <v>175</v>
       </c>
-      <c r="K35" s="271"/>
-      <c r="L35" s="272" t="s">
+      <c r="K35" s="226"/>
+      <c r="L35" s="227" t="s">
         <v>148</v>
       </c>
-      <c r="M35" s="285">
+      <c r="M35" s="240">
         <f>M34-M23</f>
         <v>185</v>
       </c>
-      <c r="N35" s="272">
+      <c r="N35" s="227">
         <f>N34-N23</f>
         <v>155</v>
       </c>
-      <c r="O35" s="273">
+      <c r="O35" s="228">
         <f>O34-O23</f>
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I36" s="274" t="s">
+      <c r="I36" s="229" t="s">
         <v>118</v>
       </c>
-      <c r="J36" s="275" t="s">
+      <c r="J36" s="230" t="s">
         <v>170</v>
       </c>
-      <c r="K36" s="276"/>
-      <c r="L36" s="277" t="s">
+      <c r="K36" s="231"/>
+      <c r="L36" s="232" t="s">
         <v>148</v>
       </c>
-      <c r="M36" s="277" t="s">
+      <c r="M36" s="232" t="s">
         <v>148</v>
       </c>
-      <c r="N36" s="278">
+      <c r="N36" s="233">
         <f>M35-M30</f>
         <v>65</v>
       </c>
-      <c r="O36" s="279">
+      <c r="O36" s="234">
         <f>N35-N30</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F37" s="195" t="s">
+      <c r="F37" s="274" t="s">
         <v>129</v>
       </c>
-      <c r="G37" s="195"/>
-      <c r="H37" s="209"/>
+      <c r="G37" s="274"/>
+      <c r="H37" s="279"/>
       <c r="I37" s="100" t="s">
         <v>121</v>
       </c>
@@ -19576,45 +19563,45 @@
         <v>122</v>
       </c>
       <c r="K37" s="2"/>
-      <c r="L37" s="282" t="s">
+      <c r="L37" s="237" t="s">
         <v>148</v>
       </c>
-      <c r="M37" s="286">
+      <c r="M37" s="241">
         <f>M25</f>
         <v>2350</v>
       </c>
-      <c r="N37" s="286">
+      <c r="N37" s="241">
         <f>N25-N36</f>
         <v>2235</v>
       </c>
-      <c r="O37" s="287">
+      <c r="O37" s="242">
         <v>2200</v>
       </c>
     </row>
     <row r="38" spans="3:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E38" s="225" t="s">
+      <c r="E38" s="269" t="s">
         <v>134</v>
       </c>
-      <c r="F38" s="225"/>
-      <c r="G38" s="225"/>
-      <c r="H38" s="225"/>
-      <c r="I38" s="203" t="s">
+      <c r="F38" s="269"/>
+      <c r="G38" s="269"/>
+      <c r="H38" s="269"/>
+      <c r="I38" s="172" t="s">
         <v>133</v>
       </c>
-      <c r="J38" s="222" t="s">
+      <c r="J38" s="186" t="s">
         <v>131</v>
       </c>
-      <c r="K38" s="203"/>
-      <c r="L38" s="204"/>
-      <c r="M38" s="223">
+      <c r="K38" s="172"/>
+      <c r="L38" s="173"/>
+      <c r="M38" s="187">
         <f>IF(M37&gt;$D$9, M37 - $D$9, 0)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="221">
+      <c r="N38" s="185">
         <f t="shared" ref="N38:O38" si="7">IF(N37&gt;$D$9, N37 - $D$9, 0)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="224">
+      <c r="O38" s="188">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -19623,30 +19610,30 @@
       <c r="I39" s="107"/>
       <c r="J39" s="107"/>
       <c r="K39" s="107"/>
-      <c r="L39" s="154" t="s">
+      <c r="L39" s="265" t="s">
         <v>92</v>
       </c>
-      <c r="M39" s="155"/>
-      <c r="N39" s="190" t="s">
+      <c r="M39" s="266"/>
+      <c r="N39" s="270" t="s">
         <v>89</v>
       </c>
-      <c r="O39" s="191"/>
+      <c r="O39" s="271"/>
     </row>
     <row r="40" spans="3:22" x14ac:dyDescent="0.3">
       <c r="I40" s="107"/>
       <c r="J40" s="107"/>
       <c r="K40" s="107"/>
-      <c r="L40" s="154"/>
-      <c r="M40" s="155"/>
-      <c r="N40" s="192"/>
-      <c r="O40" s="193"/>
+      <c r="L40" s="265"/>
+      <c r="M40" s="266"/>
+      <c r="N40" s="272"/>
+      <c r="O40" s="273"/>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.3">
       <c r="I41" s="107"/>
       <c r="J41" s="107"/>
       <c r="K41" s="107"/>
-      <c r="L41" s="156"/>
-      <c r="M41" s="157"/>
+      <c r="L41" s="267"/>
+      <c r="M41" s="268"/>
       <c r="N41" s="108"/>
       <c r="O41" s="46"/>
     </row>
@@ -19658,12 +19645,12 @@
       <c r="M42" s="46"/>
       <c r="N42" s="108"/>
       <c r="O42" s="46"/>
-      <c r="V42" s="284" t="s">
+      <c r="V42" s="239" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="43" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="V43" s="284" t="s">
+      <c r="V43" s="239" t="s">
         <v>177</v>
       </c>
     </row>
@@ -19674,7 +19661,7 @@
       <c r="C46" t="s">
         <v>124</v>
       </c>
-      <c r="D46" s="178">
+      <c r="D46" s="152">
         <v>500</v>
       </c>
       <c r="E46" t="s">
@@ -19686,7 +19673,7 @@
       <c r="C47" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="179">
+      <c r="D47" s="153">
         <v>50</v>
       </c>
       <c r="E47" t="s">
@@ -19701,7 +19688,7 @@
       <c r="C48" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="179">
+      <c r="D48" s="153">
         <v>1</v>
       </c>
       <c r="E48" t="s">
@@ -19716,7 +19703,7 @@
       <c r="C49" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="196">
+      <c r="D49" s="165">
         <v>2400</v>
       </c>
       <c r="E49" t="s">
@@ -19730,11 +19717,11 @@
     </row>
     <row r="50" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J50" s="1"/>
-      <c r="M50" s="158" t="s">
+      <c r="M50" s="252" t="s">
         <v>51</v>
       </c>
-      <c r="N50" s="159"/>
-      <c r="O50" s="160"/>
+      <c r="N50" s="253"/>
+      <c r="O50" s="254"/>
     </row>
     <row r="51" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G51" s="87" t="s">
@@ -19764,13 +19751,13 @@
       </c>
     </row>
     <row r="52" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F52" s="165" t="s">
+      <c r="F52" s="247" t="s">
         <v>56</v>
       </c>
-      <c r="G52" s="166" t="s">
+      <c r="G52" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="161" t="s">
+      <c r="H52" s="255" t="s">
         <v>9</v>
       </c>
       <c r="I52" s="135" t="s">
@@ -19798,9 +19785,9 @@
       </c>
     </row>
     <row r="53" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F53" s="165"/>
-      <c r="G53" s="167"/>
-      <c r="H53" s="162"/>
+      <c r="F53" s="247"/>
+      <c r="G53" s="249"/>
+      <c r="H53" s="256"/>
       <c r="I53" s="121" t="s">
         <v>86</v>
       </c>
@@ -19822,11 +19809,11 @@
       </c>
     </row>
     <row r="54" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F54" s="165"/>
-      <c r="G54" s="168" t="s">
+      <c r="F54" s="247"/>
+      <c r="G54" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="163" t="s">
+      <c r="H54" s="257" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="136" t="s">
@@ -19844,19 +19831,19 @@
         <f>rank_oct!$O$8</f>
         <v>310</v>
       </c>
-      <c r="N54" s="174">
+      <c r="N54" s="148">
         <f>rank_nov!$O$8</f>
         <v>300</v>
       </c>
-      <c r="O54" s="175">
+      <c r="O54" s="149">
         <f>rank_dec!$O$8</f>
         <v>360</v>
       </c>
     </row>
     <row r="55" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F55" s="165"/>
-      <c r="G55" s="167"/>
-      <c r="H55" s="162"/>
+      <c r="F55" s="247"/>
+      <c r="G55" s="249"/>
+      <c r="H55" s="256"/>
       <c r="I55" s="121" t="s">
         <v>86</v>
       </c>
@@ -19878,11 +19865,11 @@
       </c>
     </row>
     <row r="56" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F56" s="165"/>
-      <c r="G56" s="168" t="s">
+      <c r="F56" s="247"/>
+      <c r="G56" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="163" t="s">
+      <c r="H56" s="257" t="s">
         <v>11</v>
       </c>
       <c r="I56" s="136" t="s">
@@ -19900,19 +19887,19 @@
         <f>rank_oct!$O$9</f>
         <v>130</v>
       </c>
-      <c r="N56" s="174">
+      <c r="N56" s="148">
         <f>rank_nov!$O$9</f>
         <v>100</v>
       </c>
-      <c r="O56" s="175">
+      <c r="O56" s="149">
         <f>rank_dec!$O$9</f>
         <v>110</v>
       </c>
     </row>
     <row r="57" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F57" s="165"/>
-      <c r="G57" s="167"/>
-      <c r="H57" s="162"/>
+      <c r="F57" s="247"/>
+      <c r="G57" s="249"/>
+      <c r="H57" s="256"/>
       <c r="I57" s="121" t="s">
         <v>86</v>
       </c>
@@ -19934,11 +19921,11 @@
       </c>
     </row>
     <row r="58" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F58" s="165"/>
-      <c r="G58" s="168" t="s">
+      <c r="F58" s="247"/>
+      <c r="G58" s="250" t="s">
         <v>16</v>
       </c>
-      <c r="H58" s="163" t="s">
+      <c r="H58" s="257" t="s">
         <v>12</v>
       </c>
       <c r="I58" s="136" t="s">
@@ -19956,19 +19943,19 @@
         <f>rank_oct!$O$10</f>
         <v>890</v>
       </c>
-      <c r="N58" s="174">
+      <c r="N58" s="148">
         <f>rank_nov!$O$10</f>
         <v>840</v>
       </c>
-      <c r="O58" s="175">
+      <c r="O58" s="149">
         <f>rank_dec!$O$10</f>
         <v>840</v>
       </c>
     </row>
     <row r="59" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F59" s="165"/>
-      <c r="G59" s="169"/>
-      <c r="H59" s="164"/>
+      <c r="F59" s="247"/>
+      <c r="G59" s="251"/>
+      <c r="H59" s="258"/>
       <c r="I59" s="122" t="s">
         <v>86</v>
       </c>
@@ -20005,11 +19992,11 @@
         <f t="shared" ref="M60:O61" si="8">M52+M54+M56+M58</f>
         <v>2365</v>
       </c>
-      <c r="N60" s="176">
+      <c r="N60" s="150">
         <f t="shared" si="8"/>
         <v>2265</v>
       </c>
-      <c r="O60" s="177">
+      <c r="O60" s="151">
         <f t="shared" si="8"/>
         <v>2285</v>
       </c>
@@ -20021,20 +20008,20 @@
       <c r="J61" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="K61" s="184"/>
-      <c r="L61" s="185">
+      <c r="K61" s="158"/>
+      <c r="L61" s="159">
         <f>L53+L55+L57+L59</f>
         <v>2600</v>
       </c>
-      <c r="M61" s="186">
+      <c r="M61" s="160">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N61" s="186">
+      <c r="N61" s="160">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O61" s="187">
+      <c r="O61" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -20043,35 +20030,35 @@
       <c r="H62" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="I62" s="227" t="s">
+      <c r="I62" s="190" t="s">
         <v>142</v>
       </c>
-      <c r="J62" s="228" t="s">
+      <c r="J62" s="191" t="s">
         <v>120</v>
       </c>
-      <c r="K62" s="229"/>
-      <c r="L62" s="230">
+      <c r="K62" s="192"/>
+      <c r="L62" s="193">
         <v>300</v>
       </c>
-      <c r="M62" s="230">
+      <c r="M62" s="193">
         <v>200</v>
       </c>
-      <c r="N62" s="230">
+      <c r="N62" s="193">
         <v>300</v>
       </c>
-      <c r="O62" s="231">
+      <c r="O62" s="194">
         <v>200</v>
       </c>
     </row>
     <row r="63" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G63" s="152" t="s">
+      <c r="G63" s="263" t="s">
         <v>136</v>
       </c>
-      <c r="H63" s="152"/>
+      <c r="H63" s="263"/>
       <c r="I63" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J63" s="188" t="s">
+      <c r="J63" s="162" t="s">
         <v>141</v>
       </c>
       <c r="K63" s="99"/>
@@ -20093,12 +20080,12 @@
       </c>
     </row>
     <row r="64" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="G64" s="152"/>
-      <c r="H64" s="152"/>
+      <c r="G64" s="263"/>
+      <c r="H64" s="263"/>
       <c r="I64" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J64" s="216" t="s">
+      <c r="J64" s="184" t="s">
         <v>111</v>
       </c>
       <c r="K64" s="58">
@@ -20123,12 +20110,12 @@
       </c>
     </row>
     <row r="65" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G65" s="152"/>
-      <c r="H65" s="152"/>
+      <c r="G65" s="263"/>
+      <c r="H65" s="263"/>
       <c r="I65" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="J65" s="226" t="s">
+      <c r="J65" s="189" t="s">
         <v>140</v>
       </c>
       <c r="K65" s="98"/>
@@ -20150,10 +20137,10 @@
       </c>
     </row>
     <row r="66" spans="5:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G66" s="170" t="s">
+      <c r="G66" s="243" t="s">
         <v>143</v>
       </c>
-      <c r="H66" s="171"/>
+      <c r="H66" s="244"/>
       <c r="I66" s="93" t="s">
         <v>55</v>
       </c>
@@ -20161,32 +20148,32 @@
         <v>145</v>
       </c>
       <c r="K66" s="94"/>
-      <c r="L66" s="180">
+      <c r="L66" s="154">
         <f xml:space="preserve"> CEILING(L65/$D$47,1)*$D$47</f>
         <v>2300</v>
       </c>
-      <c r="M66" s="180">
+      <c r="M66" s="154">
         <f t="shared" ref="M66:O66" si="12" xml:space="preserve"> CEILING(M65/$D$47,1)*$D$47</f>
         <v>2250</v>
       </c>
-      <c r="N66" s="232">
+      <c r="N66" s="195">
         <f t="shared" si="12"/>
         <v>2350</v>
       </c>
-      <c r="O66" s="194">
+      <c r="O66" s="164">
         <f t="shared" si="12"/>
         <v>2200</v>
       </c>
     </row>
     <row r="67" spans="5:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G67" s="152" t="s">
+      <c r="G67" s="263" t="s">
         <v>138</v>
       </c>
-      <c r="H67" s="152"/>
+      <c r="H67" s="263"/>
       <c r="I67" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J67" s="188" t="s">
+      <c r="J67" s="162" t="s">
         <v>113</v>
       </c>
       <c r="K67" s="99"/>
@@ -20208,12 +20195,12 @@
       </c>
     </row>
     <row r="68" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="G68" s="152"/>
-      <c r="H68" s="152"/>
+      <c r="G68" s="263"/>
+      <c r="H68" s="263"/>
       <c r="I68" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J68" s="216" t="s">
+      <c r="J68" s="184" t="s">
         <v>114</v>
       </c>
       <c r="K68" s="58">
@@ -20238,19 +20225,19 @@
       </c>
     </row>
     <row r="69" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G69" s="152"/>
-      <c r="H69" s="152"/>
+      <c r="G69" s="263"/>
+      <c r="H69" s="263"/>
       <c r="I69" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="J69" s="226" t="s">
+      <c r="J69" s="189" t="s">
         <v>139</v>
       </c>
       <c r="K69" s="98"/>
-      <c r="L69" s="235" t="s">
+      <c r="L69" s="198" t="s">
         <v>148</v>
       </c>
-      <c r="M69" s="235" t="s">
+      <c r="M69" s="198" t="s">
         <v>148</v>
       </c>
       <c r="N69" s="23">
@@ -20263,10 +20250,10 @@
       </c>
     </row>
     <row r="70" spans="5:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G70" s="170" t="s">
+      <c r="G70" s="243" t="s">
         <v>144</v>
       </c>
-      <c r="H70" s="171"/>
+      <c r="H70" s="244"/>
       <c r="I70" s="93" t="s">
         <v>55</v>
       </c>
@@ -20274,19 +20261,19 @@
         <v>146</v>
       </c>
       <c r="K70" s="94"/>
-      <c r="L70" s="180">
+      <c r="L70" s="154">
         <f>L66</f>
         <v>2300</v>
       </c>
-      <c r="M70" s="180">
+      <c r="M70" s="154">
         <f>M66</f>
         <v>2250</v>
       </c>
-      <c r="N70" s="233">
+      <c r="N70" s="196">
         <f xml:space="preserve"> CEILING(N69/$D$47,1)*$D$47</f>
         <v>2500</v>
       </c>
-      <c r="O70" s="194">
+      <c r="O70" s="164">
         <f xml:space="preserve"> CEILING(O69/$D$47,1)*$D$47</f>
         <v>2200</v>
       </c>
@@ -20298,65 +20285,65 @@
       <c r="J71" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="K71" s="181"/>
-      <c r="L71" s="234">
+      <c r="K71" s="155"/>
+      <c r="L71" s="197">
         <f>M70</f>
         <v>2250</v>
       </c>
-      <c r="M71" s="182">
+      <c r="M71" s="156">
         <f t="shared" ref="M71:O71" si="16">N70</f>
         <v>2500</v>
       </c>
-      <c r="N71" s="182">
+      <c r="N71" s="156">
         <f t="shared" si="16"/>
         <v>2200</v>
       </c>
-      <c r="O71" s="183">
+      <c r="O71" s="157">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E72" s="225" t="s">
+      <c r="E72" s="269" t="s">
         <v>134</v>
       </c>
-      <c r="F72" s="225"/>
-      <c r="G72" s="225"/>
-      <c r="H72" s="225"/>
-      <c r="I72" s="203" t="s">
+      <c r="F72" s="269"/>
+      <c r="G72" s="269"/>
+      <c r="H72" s="269"/>
+      <c r="I72" s="172" t="s">
         <v>133</v>
       </c>
-      <c r="J72" s="222" t="s">
+      <c r="J72" s="186" t="s">
         <v>131</v>
       </c>
-      <c r="K72" s="203"/>
-      <c r="L72" s="204"/>
-      <c r="M72" s="223">
+      <c r="K72" s="172"/>
+      <c r="L72" s="173"/>
+      <c r="M72" s="187">
         <f>IF(M70&gt;$D$49, M70 - $D$49, 0)</f>
         <v>0</v>
       </c>
-      <c r="N72" s="221">
+      <c r="N72" s="185">
         <f>IF(N70&gt;$D$49, N70 - $D$49, 0)</f>
         <v>100</v>
       </c>
-      <c r="O72" s="224">
+      <c r="O72" s="188">
         <f>IF(O70&gt;$D$49, O70 - $D$49, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="L73" s="154" t="s">
+      <c r="L73" s="265" t="s">
         <v>92</v>
       </c>
-      <c r="M73" s="155"/>
+      <c r="M73" s="266"/>
     </row>
     <row r="74" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="L74" s="154"/>
-      <c r="M74" s="155"/>
+      <c r="L74" s="265"/>
+      <c r="M74" s="266"/>
     </row>
     <row r="75" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="L75" s="156"/>
-      <c r="M75" s="157"/>
+      <c r="L75" s="267"/>
+      <c r="M75" s="268"/>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
@@ -20444,6 +20431,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="N39:O40"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="F15:F22"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="L39:M41"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H58:H59"/>
     <mergeCell ref="L73:M75"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="F25:H25"/>
@@ -20460,24 +20465,6 @@
     <mergeCell ref="G52:G53"/>
     <mergeCell ref="H52:H53"/>
     <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="N39:O40"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="F15:F22"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="L39:M41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20767,7 +20754,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>